<commit_message>
Añadido README y PPT para presentación
</commit_message>
<xml_diff>
--- a/documentacion/Plantilla de historias de usuario y seguimiento del proyecto.xlsx
+++ b/documentacion/Plantilla de historias de usuario y seguimiento del proyecto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efatu\Desktop\Proyecto Final DAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efatu\Desktop\Proyecto Final DAM\proyecto-final\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7DAE46-3E89-47BA-9E3A-9A174C9FB88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A6789-FCE2-4182-8D22-E925DBEB66CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
   <si>
     <t>Proyecto</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Puntos Estimados</t>
   </si>
   <si>
-    <t xml:space="preserve">Horas empleadas </t>
-  </si>
-  <si>
-    <t>Rama / Hash commit</t>
-  </si>
-  <si>
     <t>HU-01</t>
   </si>
   <si>
@@ -167,9 +161,6 @@
     <t>Como usuario quiero poder hacer login en la app</t>
   </si>
   <si>
-    <t>Como usuario quiero poder hacer registrarme en la app</t>
-  </si>
-  <si>
     <t>Como admin quiero poder dar de alta un sitio de cualquier tipo</t>
   </si>
   <si>
@@ -188,21 +179,6 @@
     <t>Como propietario del sitio o admin quiero poder eliminar mi sitio, identificado por su ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Como admin quiero poder añadir la información de un servicio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como admin quiero poder editar la información de un servicio </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como admin quiero poder eliminar un servicio </t>
-  </si>
-  <si>
-    <t>Como admin o propietario de un sitio quiero poder listar todos los servicios disponibles</t>
-  </si>
-  <si>
-    <t>Como admin o propietario de un sitio quiero poder mostrar la información de un servicio, identificado por su ID</t>
-  </si>
-  <si>
     <t>Como usuario quiero poder pedir cita en un sitio</t>
   </si>
   <si>
@@ -255,6 +231,102 @@
   </si>
   <si>
     <t>Como usuario quiero poder ver mis sitios favoritos</t>
+  </si>
+  <si>
+    <t>Nos logueamos correctamente en la app</t>
+  </si>
+  <si>
+    <t>Podemos registrarnos correctamente</t>
+  </si>
+  <si>
+    <t>Creamos un nuevo negocio</t>
+  </si>
+  <si>
+    <t>Se listan los negocios existentes</t>
+  </si>
+  <si>
+    <t>Se muestran los negocios de un tipo concreto</t>
+  </si>
+  <si>
+    <t>Se muestra la información de un negocio por su ID</t>
+  </si>
+  <si>
+    <t>Se actualiza correctamente la información de un negocio</t>
+  </si>
+  <si>
+    <t>Se elimina el negocio deseado</t>
+  </si>
+  <si>
+    <t>Se añade la cita al usuario y al negocio seleccionado</t>
+  </si>
+  <si>
+    <t>Se edita la información de una cita</t>
+  </si>
+  <si>
+    <t>Se muestra el listado de las citas</t>
+  </si>
+  <si>
+    <t>Se muestra la información de una cita por su ID</t>
+  </si>
+  <si>
+    <t>Se elimina la cita del usuario y del negocio</t>
+  </si>
+  <si>
+    <t>Se añade el comentario al negocio seleccionado</t>
+  </si>
+  <si>
+    <t>Se actualiza correctamente la información de un comentario</t>
+  </si>
+  <si>
+    <t>Se listan todos los comentarios</t>
+  </si>
+  <si>
+    <t>Se muestra la información de un comentario</t>
+  </si>
+  <si>
+    <t>Se elimina un comentario</t>
+  </si>
+  <si>
+    <t>Se elimina el comentario</t>
+  </si>
+  <si>
+    <t>Se añade el negocio a mi lista de favoritos</t>
+  </si>
+  <si>
+    <t>Se elimina el negocio de mis sitios favoritos</t>
+  </si>
+  <si>
+    <t>Se listan los negocios marcados como favoritos</t>
+  </si>
+  <si>
+    <t>Como usuario quiero filtar los negocios por la contención de una cadena de texto concreta relativa al nombre de dicho negocio</t>
+  </si>
+  <si>
+    <t>Como usuario quiero filtar los negocios por su tipo</t>
+  </si>
+  <si>
+    <t>Se filtran correctamente los negocios</t>
+  </si>
+  <si>
+    <t>Como usuario quiero filtar los negocios por su ciudad</t>
+  </si>
+  <si>
+    <t>Como usuario quiero filtar los negocios por su código postal</t>
+  </si>
+  <si>
+    <t>Como usuario quiero filtar los negocios por su propietario</t>
+  </si>
+  <si>
+    <t>HU-29</t>
+  </si>
+  <si>
+    <t>Como usuario quiero conocer si una hora está disponible para pedir cita</t>
+  </si>
+  <si>
+    <t>Se muestra verdadero o falso según exista ya una cita con la hora seleccionada</t>
+  </si>
+  <si>
+    <t>Como usuario quiero poder hacer registrarme en la app, independientemente del rol que tenga</t>
   </si>
 </sst>
 </file>
@@ -409,19 +481,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -432,6 +501,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,10 +759,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J998"/>
+  <dimension ref="A1:H993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,53 +773,52 @@
     <col min="4" max="4" width="46.5546875" customWidth="1"/>
     <col min="5" max="7" width="20.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="47.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="11"/>
@@ -757,650 +828,655 @@
       <c r="H9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>47</v>
+      <c r="C10" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>50</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="F13" s="11"/>
       <c r="G13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="F14" s="11"/>
       <c r="G14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>52</v>
+        <v>11</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="13"/>
       <c r="G15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>53</v>
+        <v>11</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="E16" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>54</v>
+        <v>11</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H17" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>55</v>
+        <v>11</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="D18" s="11"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="F18" s="11"/>
       <c r="G18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H18" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>58</v>
+        <v>11</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="D19" s="11"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>59</v>
+        <v>11</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="10"/>
+      <c r="E20" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H20" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D21" s="11"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H21" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="G22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="D23" s="11"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H23" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>61</v>
+        <v>11</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="F24" s="11"/>
       <c r="G24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H24" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="D25" s="11"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H25" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="F26" s="11"/>
       <c r="G26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H26" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="F27" s="11"/>
       <c r="G27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H27" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>65</v>
+        <v>11</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="F28" s="11"/>
       <c r="G28" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H28" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>66</v>
+        <v>11</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D29" s="11"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="12" t="s">
+        <v>88</v>
+      </c>
       <c r="F29" s="11"/>
       <c r="G29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H29" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>68</v>
+        <v>11</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="F30" s="11"/>
       <c r="G30" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="9"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H30" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>67</v>
+        <v>11</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="D31" s="11"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="F31" s="11"/>
       <c r="G31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="9"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H31" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="F32" s="11"/>
       <c r="G32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="9"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H32" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="D33" s="11"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F33" s="11"/>
       <c r="G33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H33" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D34" s="11"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F34" s="11"/>
       <c r="G34" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="9"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H34" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D35" s="11"/>
-      <c r="E35" s="10"/>
+      <c r="E35" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F35" s="11"/>
       <c r="G35" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="9"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H35" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="D36" s="11"/>
-      <c r="E36" s="10"/>
+      <c r="E36" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F36" s="11"/>
       <c r="G36" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="D37" s="11"/>
-      <c r="E37" s="10"/>
+      <c r="E37" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F37" s="11"/>
       <c r="G37" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="9"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="H37" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>99</v>
+      </c>
       <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
+      <c r="E38" s="10" t="s">
+        <v>100</v>
+      </c>
       <c r="F38" s="11"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G38" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2346,103 +2422,88 @@
     <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
+  <mergeCells count="62">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="G10:G43">
+  <conditionalFormatting sqref="G10:G38">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Terminada"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G43">
+  <conditionalFormatting sqref="G10:G38">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"No iniciada"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G43">
+  <conditionalFormatting sqref="G10:G38">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"En progreso"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10:G43">
+  <conditionalFormatting sqref="G10:G38">
     <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"En pruebas"</formula>
     </cfRule>
@@ -2455,13 +2516,13 @@
           <x14:formula1>
             <xm:f>Datamaster!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B10:B43</xm:sqref>
+          <xm:sqref>B10:B38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Datamaster!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G10:G43</xm:sqref>
+          <xm:sqref>G10:G38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2486,36 +2547,36 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>